<commit_message>
commit after firefox worked, but cant work with other keywords
</commit_message>
<xml_diff>
--- a/src/com/qtpselenium/xls/C Suite.xlsx
+++ b/src/com/qtpselenium/xls/C Suite.xlsx
@@ -10,13 +10,15 @@
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
     <sheet name="Test Steps" sheetId="2" r:id="rId2"/>
     <sheet name="SampleTest" sheetId="3" r:id="rId3"/>
+    <sheet name="selectTest" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="69">
   <si>
     <t>TCID</t>
   </si>
@@ -69,9 +71,6 @@
     <t>Forgot_passwd_linktext</t>
   </si>
   <si>
-    <t>data</t>
-  </si>
-  <si>
     <t>object</t>
   </si>
   <si>
@@ -154,12 +153,85 @@
   </si>
   <si>
     <t>config|TestURL</t>
+  </si>
+  <si>
+    <t>selectTest</t>
+  </si>
+  <si>
+    <t>selectList</t>
+  </si>
+  <si>
+    <t>city_list</t>
+  </si>
+  <si>
+    <t>col|City</t>
+  </si>
+  <si>
+    <t>verifyListSelection</t>
+  </si>
+  <si>
+    <t>closeBrowser</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>Newyork</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>config+TestURL</t>
+  </si>
+  <si>
+    <t>config/browserType</t>
+  </si>
+  <si>
+    <t>sheet2</t>
+  </si>
+  <si>
+    <t>config=browserType</t>
+  </si>
+  <si>
+    <t>config=TestURL</t>
+  </si>
+  <si>
+    <t>Result2</t>
+  </si>
+  <si>
+    <t>Result3</t>
+  </si>
+  <si>
+    <t>Result4</t>
+  </si>
+  <si>
+    <t>Result5</t>
+  </si>
+  <si>
+    <t>verifyText</t>
+  </si>
+  <si>
+    <t>col=Username</t>
+  </si>
+  <si>
+    <t>Object</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>FAIL--- Exception occured. Not able to Verify Button Text</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -215,12 +287,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -518,14 +595,14 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="25.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="25.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="25.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -560,26 +637,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="H2" sqref="H2:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" style="4" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="26.140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="21.85546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="26.7109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="7.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="4" width="13.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="26.140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="21.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="26.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="7.5154296875" collapsed="true"/>
+    <col min="9" max="12" bestFit="true" customWidth="true" width="7.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:12">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -593,10 +670,10 @@
         <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>18</v>
+        <v>66</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>17</v>
+        <v>54</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>9</v>
@@ -604,8 +681,20 @@
       <c r="H1" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="I1" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -613,10 +702,13 @@
         <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+        <v>58</v>
+      </c>
+      <c r="H2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -624,107 +716,27 @@
         <v>11</v>
       </c>
       <c r="F3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+        <v>59</v>
+      </c>
+      <c r="H3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>64</v>
       </c>
       <c r="E4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" t="s">
-        <v>35</v>
-      </c>
-      <c r="F6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F7" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="F4" t="s">
         <v>38</v>
       </c>
-      <c r="F9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" t="s">
-        <v>34</v>
+      <c r="H4" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -738,43 +750,43 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.28515625" customWidth="1"/>
-    <col min="3" max="3" width="29.42578125" customWidth="1"/>
-    <col min="4" max="4" width="22.5703125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="29.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="22.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D2" t="s">
         <v>5</v>
@@ -785,58 +797,349 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" t="s">
         <v>30</v>
       </c>
-      <c r="B3" t="s">
-        <v>31</v>
-      </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E3" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="C4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E4" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="B5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E5" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" t="s">
         <v>43</v>
       </c>
-      <c r="D6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" t="s">
-        <v>5</v>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="4"/>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" t="s">
+        <v>64</v>
+      </c>
+      <c r="E19" t="s">
+        <v>37</v>
+      </c>
+      <c r="F19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" t="s">
+        <v>18</v>
+      </c>
+      <c r="E20" t="s">
+        <v>34</v>
+      </c>
+      <c r="F20" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>